<commit_message>
Add 2019 cover and density data
fixing plot numbering issues
move veg height data to sedgwickenv package
fixing species name issues
</commit_message>
<xml_diff>
--- a/data-raw/cover_2019/745_wholeplot.xlsx
+++ b/data-raw/cover_2019/745_wholeplot.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy/Dropbox/projects/sedgwickcover/data-raw/cover_2019/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB54F70-1ED8-8846-9D29-5C74F2C00E34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="7320" yWindow="2140" windowWidth="38400" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -94,77 +103,388 @@
     <t>CRCO</t>
   </si>
   <si>
-    <t>ERIO</t>
-  </si>
-  <si>
     <t>POSE</t>
   </si>
   <si>
     <t>CHPA</t>
+  </si>
+  <si>
+    <t>ERIOGONUM_BIG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -214,766 +534,766 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="H2" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J2" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2">
-        <v>415.0</v>
+        <v>415</v>
       </c>
       <c r="H3" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="J3" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>134.0</v>
+        <v>134</v>
       </c>
       <c r="F4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="J4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="2">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I6" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J6" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K6" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I7" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="J7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="2">
-        <v>39.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="H8" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I8" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J8" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K8" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F9" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G9" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="H9" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I9" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="J9" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I10" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J10" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="2">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="F11" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="H11" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="J11" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="2">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F12" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H12" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J13" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I14" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="J14" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C16" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H17" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I17" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J17" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H18" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F20" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I20" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I21" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J21" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H22" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J22" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K22" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K23" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K24" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H25" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="2">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="J25" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="I26" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="s">
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="I27" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="J27" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K27" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J28" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>